<commit_message>
Thắng lên tiến độ
</commit_message>
<xml_diff>
--- a/2015/201510/20_MANAGEMENT/SOF.QP.03.F05_TaskList.xlsx
+++ b/2015/201510/20_MANAGEMENT/SOF.QP.03.F05_TaskList.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2160"/>
@@ -10,8 +10,8 @@
     <sheet name="Tasks" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -293,7 +293,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -333,6 +333,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -354,12 +363,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -369,8 +372,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -742,18 +748,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -767,12 +773,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16" t="s">
+      <c r="A1" s="18"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="17"/>
+      <c r="D1" s="20"/>
       <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
@@ -781,20 +787,20 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="4" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="19"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="22"/>
       <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" s="4" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="21"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
       <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
@@ -808,33 +814,33 @@
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="36.75" customHeight="1">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="15" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="16" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="25" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="12"/>
@@ -842,233 +848,255 @@
       <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A7" s="23"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="25"/>
+      <c r="C7" s="26"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="16" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="25"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A9" s="23"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="25"/>
+      <c r="C9" s="26"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="25"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A11" s="23"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="25"/>
+      <c r="C11" s="26"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="25"/>
+      <c r="C12" s="26"/>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A13" s="23"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="25"/>
+      <c r="C13" s="26"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="16" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="25"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
     </row>
     <row r="15" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A15" s="23"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="25"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="25"/>
+      <c r="C16" s="26"/>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
     </row>
     <row r="17" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A17" s="23"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="25"/>
+      <c r="C17" s="26"/>
       <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
+      <c r="E17" s="28">
+        <v>5</v>
+      </c>
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="16" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="25"/>
+      <c r="C18" s="26"/>
       <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
+      <c r="E18" s="28">
+        <v>2</v>
+      </c>
       <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A19" s="23"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="25"/>
+      <c r="C19" s="26"/>
       <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
+      <c r="E19" s="28">
+        <v>3</v>
+      </c>
       <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="16" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="25"/>
+      <c r="C20" s="26"/>
       <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
+      <c r="E20" s="28">
+        <v>2</v>
+      </c>
       <c r="F20" s="12"/>
     </row>
     <row r="21" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A21" s="23"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="25"/>
+      <c r="C21" s="26"/>
       <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
+      <c r="E21" s="28">
+        <v>4</v>
+      </c>
       <c r="F21" s="12"/>
     </row>
     <row r="22" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="25"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
+      <c r="E22" s="28">
+        <v>2</v>
+      </c>
       <c r="F22" s="12"/>
     </row>
     <row r="23" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A23" s="23"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="25"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
+      <c r="E23" s="28">
+        <v>6</v>
+      </c>
       <c r="F23" s="12"/>
     </row>
     <row r="24" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="16" t="s">
         <v>20</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="25"/>
+      <c r="C24" s="26"/>
       <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
+      <c r="E24" s="28">
+        <v>2</v>
+      </c>
       <c r="F24" s="12"/>
     </row>
     <row r="25" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A25" s="23"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="25"/>
+      <c r="C25" s="26"/>
       <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
+      <c r="E25" s="28">
+        <v>4</v>
+      </c>
       <c r="F25" s="12"/>
     </row>
     <row r="26" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="25"/>
+      <c r="C26" s="26"/>
       <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
+      <c r="E26" s="28">
+        <v>3</v>
+      </c>
       <c r="F26" s="12"/>
     </row>
     <row r="27" spans="1:6" ht="15">
-      <c r="A27" s="23"/>
+      <c r="A27" s="17"/>
       <c r="B27" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="26"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="9"/>
+      <c r="E27" s="29">
+        <v>7</v>
+      </c>
       <c r="F27" s="9"/>
     </row>
     <row r="28" spans="1:6" ht="15">
@@ -1153,6 +1181,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:B3"/>
+    <mergeCell ref="C1:D3"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="C6:C27"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A14:A15"/>
@@ -1160,13 +1195,6 @@
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A1:B3"/>
-    <mergeCell ref="C1:D3"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="C6:C27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Dự trù dùm anh thời gian sẽ hoàn thành các task
</commit_message>
<xml_diff>
--- a/2015/201510/20_MANAGEMENT/SOF.QP.03.F05_TaskList.xlsx
+++ b/2015/201510/20_MANAGEMENT/SOF.QP.03.F05_TaskList.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\THUC TAP\SVN_Test\20_MANAGEMENT\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2160"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -336,33 +341,39 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -371,12 +382,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -748,7 +753,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -759,7 +764,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -834,267 +839,300 @@
       </c>
     </row>
     <row r="6" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="25" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="27" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
+      <c r="E6" s="16">
+        <f xml:space="preserve"> 20*0.3</f>
+        <v>6</v>
+      </c>
       <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A7" s="17"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="26"/>
+      <c r="C7" s="28"/>
       <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
+      <c r="E7" s="16">
+        <f>12*0.3</f>
+        <v>3.5999999999999996</v>
+      </c>
       <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="25" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="26"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
+      <c r="E8" s="16">
+        <f xml:space="preserve"> 12*0.3</f>
+        <v>3.5999999999999996</v>
+      </c>
       <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A9" s="17"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="26"/>
+      <c r="C9" s="28"/>
       <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
+      <c r="E9" s="16">
+        <f>26*0.3</f>
+        <v>7.8</v>
+      </c>
       <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="25" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="26"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
+      <c r="E10" s="16">
+        <f>16*0.3</f>
+        <v>4.8</v>
+      </c>
       <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A11" s="17"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="26"/>
+      <c r="C11" s="28"/>
       <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
+      <c r="E11" s="16">
+        <f>20*0.3</f>
+        <v>6</v>
+      </c>
       <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="25" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="26"/>
+      <c r="C12" s="28"/>
       <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
+      <c r="E12" s="16">
+        <f>14*0.3</f>
+        <v>4.2</v>
+      </c>
       <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A13" s="17"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="26"/>
+      <c r="C13" s="28"/>
       <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
+      <c r="E13" s="16">
+        <f>30*0.3</f>
+        <v>9</v>
+      </c>
       <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="26"/>
+      <c r="C14" s="28"/>
       <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
+      <c r="E14" s="16">
+        <f>18*0.3</f>
+        <v>5.3999999999999995</v>
+      </c>
       <c r="F14" s="12"/>
     </row>
     <row r="15" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A15" s="17"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="26"/>
+      <c r="C15" s="28"/>
       <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
+      <c r="E15" s="16">
+        <f>22*0.3</f>
+        <v>6.6</v>
+      </c>
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="25" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="26"/>
+      <c r="C16" s="28"/>
       <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
+      <c r="E16" s="16">
+        <f>14*0.3</f>
+        <v>4.2</v>
+      </c>
       <c r="F16" s="12"/>
     </row>
     <row r="17" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A17" s="17"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="26"/>
+      <c r="C17" s="28"/>
       <c r="D17" s="12"/>
-      <c r="E17" s="28">
+      <c r="E17" s="16">
         <v>5</v>
       </c>
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="25" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="26"/>
+      <c r="C18" s="28"/>
       <c r="D18" s="12"/>
-      <c r="E18" s="28">
+      <c r="E18" s="16">
         <v>2</v>
       </c>
       <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A19" s="17"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="26"/>
+      <c r="C19" s="28"/>
       <c r="D19" s="12"/>
-      <c r="E19" s="28">
+      <c r="E19" s="16">
         <v>3</v>
       </c>
       <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="25" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="26"/>
+      <c r="C20" s="28"/>
       <c r="D20" s="12"/>
-      <c r="E20" s="28">
+      <c r="E20" s="16">
         <v>2</v>
       </c>
       <c r="F20" s="12"/>
     </row>
     <row r="21" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A21" s="17"/>
+      <c r="A21" s="26"/>
       <c r="B21" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="26"/>
+      <c r="C21" s="28"/>
       <c r="D21" s="12"/>
-      <c r="E21" s="28">
+      <c r="E21" s="16">
         <v>4</v>
       </c>
       <c r="F21" s="12"/>
     </row>
     <row r="22" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="25" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="26"/>
+      <c r="C22" s="28"/>
       <c r="D22" s="12"/>
-      <c r="E22" s="28">
+      <c r="E22" s="16">
         <v>2</v>
       </c>
       <c r="F22" s="12"/>
     </row>
     <row r="23" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A23" s="17"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="26"/>
+      <c r="C23" s="28"/>
       <c r="D23" s="12"/>
-      <c r="E23" s="28">
+      <c r="E23" s="16">
         <v>6</v>
       </c>
       <c r="F23" s="12"/>
     </row>
     <row r="24" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="25" t="s">
         <v>20</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="26"/>
+      <c r="C24" s="28"/>
       <c r="D24" s="12"/>
-      <c r="E24" s="28">
+      <c r="E24" s="16">
         <v>2</v>
       </c>
       <c r="F24" s="12"/>
     </row>
     <row r="25" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A25" s="17"/>
+      <c r="A25" s="26"/>
       <c r="B25" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="26"/>
+      <c r="C25" s="28"/>
       <c r="D25" s="12"/>
-      <c r="E25" s="28">
+      <c r="E25" s="16">
         <v>4</v>
       </c>
       <c r="F25" s="12"/>
     </row>
     <row r="26" spans="1:6" s="13" customFormat="1" ht="15">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="25" t="s">
         <v>21</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="26"/>
+      <c r="C26" s="28"/>
       <c r="D26" s="12"/>
-      <c r="E26" s="28">
+      <c r="E26" s="16">
         <v>3</v>
       </c>
       <c r="F26" s="12"/>
     </row>
     <row r="27" spans="1:6" ht="15">
-      <c r="A27" s="17"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="27"/>
+      <c r="C27" s="29"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="29">
+      <c r="E27" s="17">
         <v>7</v>
       </c>
       <c r="F27" s="9"/>

</xml_diff>